<commit_message>
add sqlite and inserted rows
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Row</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t xml:space="preserve">JJ150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Faulty</t>
   </si>
   <si>
     <t xml:space="preserve">JM101</t>
@@ -96,6 +99,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -117,6 +121,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -161,16 +166,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,107 +208,107 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="3" t="n">
         <v>41092</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="2" t="n">
         <v>101</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="3" t="n">
         <v>41092</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="2" t="n">
         <v>104</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="3" t="n">
         <v>41092</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="2" t="n">
         <v>234</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="3" t="n">
         <v>41092</v>
       </c>
     </row>
@@ -319,22 +328,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
the check is working. some minor fixes ;
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="c60 db" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Row</t>
   </si>
@@ -66,15 +66,6 @@
   </si>
   <si>
     <t xml:space="preserve">jj7654321</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jj100 devices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JJ100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JJ150</t>
   </si>
   <si>
     <t xml:space="preserve">Faulty</t>
@@ -200,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -292,26 +283,6 @@
         <v>41092</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>234</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="3" t="n">
-        <v>41092</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -330,7 +301,7 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -338,17 +309,17 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>